<commit_message>
create item and delete item working
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7770" activeTab="4"/>
+    <workbookView windowWidth="19485" windowHeight="7770" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Schema Design" sheetId="3" r:id="rId3"/>
     <sheet name="Task Details" sheetId="4" r:id="rId4"/>
     <sheet name="Links" sheetId="5" r:id="rId5"/>
+    <sheet name="Learning" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
   <si>
     <t>Todo:</t>
   </si>
@@ -339,6 +340,18 @@
   </si>
   <si>
     <t>https://www.styiens.com/</t>
+  </si>
+  <si>
+    <t>implement redux</t>
+  </si>
+  <si>
+    <t>node backend to link with redux</t>
+  </si>
+  <si>
+    <t>authentication and generating tokens</t>
+  </si>
+  <si>
+    <t>responsive design</t>
   </si>
 </sst>
 </file>
@@ -346,10 +359,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -377,7 +390,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,6 +411,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -399,16 +426,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,7 +464,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,71 +518,12 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -527,37 +540,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,145 +696,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,6 +745,39 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -770,16 +816,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,182 +846,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2051,7 +2064,7 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2084,4 +2097,44 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="28.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Create and Delete for items
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7770" activeTab="5"/>
+    <workbookView windowWidth="19485" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -135,6 +135,9 @@
     <t>copy to clipboard button</t>
   </si>
   <si>
+    <t>node APIS fix</t>
+  </si>
+  <si>
     <t>Backlog</t>
   </si>
   <si>
@@ -340,9 +343,6 @@
   </si>
   <si>
     <t>https://www.styiens.com/</t>
-  </si>
-  <si>
-    <t>implement redux</t>
   </si>
   <si>
     <t>node backend to link with redux</t>
@@ -359,10 +359,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -381,23 +381,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,35 +410,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -455,11 +418,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -478,32 +440,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,12 +472,58 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -540,187 +540,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,24 +749,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -778,21 +760,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -812,11 +779,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -832,16 +814,34 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -851,148 +851,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1363,10 +1363,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C48"/>
+  <dimension ref="A2:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1550,6 +1550,11 @@
     <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1576,15 +1581,15 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="3:3">
@@ -1644,228 +1649,228 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1905,13 +1910,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1919,10 +1924,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1930,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1938,7 +1943,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1946,7 +1951,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1954,7 +1959,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1962,7 +1967,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1970,7 +1975,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1978,15 +1983,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1994,7 +1999,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2002,12 +2007,12 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2015,10 +2020,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2026,7 +2031,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2034,7 +2039,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2042,7 +2047,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2050,7 +2055,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2076,18 +2081,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2102,10 +2107,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
@@ -2113,11 +2118,6 @@
     <col min="1" max="1" width="28.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Rendering Menu and cart components
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7770" activeTab="1"/>
+    <workbookView windowWidth="19485" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
   <si>
     <t>Todo:</t>
   </si>
@@ -138,6 +138,21 @@
     <t>node APIS fix</t>
   </si>
   <si>
+    <t>price range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort order up and down arrow </t>
+  </si>
+  <si>
+    <t>category add selection dropdown</t>
+  </si>
+  <si>
+    <t>in view add update button and delete button</t>
+  </si>
+  <si>
+    <t>pagination for items</t>
+  </si>
+  <si>
     <t>Backlog</t>
   </si>
   <si>
@@ -228,7 +243,7 @@
     <t>service</t>
   </si>
   <si>
-    <t>orders</t>
+    <t>orders[]</t>
   </si>
   <si>
     <t>address</t>
@@ -363,9 +378,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -385,6 +400,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -399,48 +429,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -452,25 +444,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -491,9 +467,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -506,27 +535,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -543,181 +558,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,21 +782,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -791,17 +791,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,11 +819,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -841,11 +835,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -854,148 +869,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1366,10 +1381,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C50"/>
+  <dimension ref="A2:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1560,6 +1575,31 @@
         <v>38</v>
       </c>
     </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1572,7 +1612,7 @@
   <sheetPr/>
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1584,15 +1624,15 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="3:3">
@@ -1628,7 +1668,7 @@
     </row>
     <row r="9" spans="3:3">
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1643,8 +1683,8 @@
   <sheetPr/>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -1657,228 +1697,228 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1910,7 +1950,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1918,13 +1958,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1932,10 +1972,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1943,7 +1983,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1951,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1959,7 +1999,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1967,7 +2007,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1975,7 +2015,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1983,7 +2023,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1991,15 +2031,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2007,7 +2047,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2015,12 +2055,12 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2028,10 +2068,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2039,7 +2079,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2047,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2055,7 +2095,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2063,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2089,18 +2129,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2128,17 +2168,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added authentication with flaws
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7770" activeTab="2"/>
+    <workbookView windowWidth="19485" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="122">
   <si>
     <t>Todo:</t>
   </si>
@@ -153,6 +153,12 @@
     <t>pagination for items</t>
   </si>
   <si>
+    <t>needs work and testing</t>
+  </si>
+  <si>
+    <t>working fine</t>
+  </si>
+  <si>
     <t>Backlog</t>
   </si>
   <si>
@@ -163,6 +169,15 @@
   </si>
   <si>
     <t>CRUD for items</t>
+  </si>
+  <si>
+    <t>Authentication:</t>
+  </si>
+  <si>
+    <t>create the Sign Up form</t>
+  </si>
+  <si>
+    <t>get data from the form</t>
   </si>
   <si>
     <t>Backend Design (Schema Design)</t>
@@ -377,10 +392,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -400,91 +415,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -507,14 +445,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -529,7 +506,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -537,13 +521,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -552,25 +567,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,163 +759,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,61 +788,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -864,167 +835,223 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1383,7 +1410,7 @@
   <sheetPr/>
   <dimension ref="A2:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -1400,56 +1427,56 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
@@ -1610,10 +1637,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:C9"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1622,53 +1649,80 @@
     <col min="3" max="3" width="41.1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
-      <c r="B1" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
-      <c r="C2" s="2" t="s">
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="3:3">
-      <c r="C3" s="3" t="s">
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3">
+      <c r="C13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="3:3">
-      <c r="C4" s="3" t="s">
+    <row r="15" spans="3:3">
+      <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+    <row r="16" spans="2:3">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
-      <c r="C6" s="3" t="s">
+    <row r="17" spans="3:3">
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="3:3">
-      <c r="C7" s="3" t="s">
+    <row r="18" spans="3:3">
+      <c r="C18" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
-      <c r="B8" t="s">
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="3:3">
-      <c r="C9" s="3" t="s">
-        <v>47</v>
+    <row r="20" spans="3:3">
+      <c r="C20" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +1737,7 @@
   <sheetPr/>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1697,228 +1751,228 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1950,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1958,13 +2012,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1972,10 +2026,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1983,7 +2037,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1991,7 +2045,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1999,7 +2053,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2007,7 +2061,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2015,7 +2069,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2023,7 +2077,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2031,15 +2085,15 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2047,7 +2101,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2055,12 +2109,12 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2068,10 +2122,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2079,7 +2133,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2087,7 +2141,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2095,7 +2149,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2103,7 +2157,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2129,18 +2183,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2168,17 +2222,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created bill generation for diwali orders
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7770" activeTab="1"/>
+    <workbookView windowWidth="19410" windowHeight="7770" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
   <si>
     <t>Todo:</t>
   </si>
@@ -294,6 +294,9 @@
     <t>Favourites</t>
   </si>
   <si>
+    <t>In progress</t>
+  </si>
+  <si>
     <t>Requirements and Analysis</t>
   </si>
   <si>
@@ -376,6 +379,28 @@
   </si>
   <si>
     <t>https://www.styiens.com/</t>
+  </si>
+  <si>
+    <t>Front end template</t>
+  </si>
+  <si>
+    <t>http://themes.templatescoder.com/pizzon/html/demo/1-0/</t>
+  </si>
+  <si>
+    <t>https://freshdesignweb.com/free-restaurant-coffee-website-templates/</t>
+  </si>
+  <si>
+    <t>Ecommerse site</t>
+  </si>
+  <si>
+    <t>http://demo.activeitzone.com/ecommerce/categories</t>
+  </si>
+  <si>
+    <t>The Credentials are 
+Seller username : seller@example.com
+Customer  username : customer@example.com
+Admin username :  admin@example.com
+password : 123456</t>
   </si>
   <si>
     <t>node backend to link with redux</t>
@@ -393,14 +418,37 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -414,22 +462,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -437,7 +479,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -452,14 +494,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -469,14 +541,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,31 +561,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -534,29 +575,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -567,49 +599,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,145 +785,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -788,11 +820,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -801,7 +839,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -817,6 +855,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -862,21 +909,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -890,162 +922,174 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1410,7 +1454,7 @@
   <sheetPr/>
   <dimension ref="A2:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -1422,64 +1466,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1494,7 +1538,7 @@
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1534,13 +1578,13 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1563,7 +1607,7 @@
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1639,8 +1683,8 @@
   <sheetPr/>
   <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1650,13 +1694,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="5"/>
       <c r="B2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="6"/>
       <c r="B3" t="s">
         <v>45</v>
       </c>
@@ -1670,33 +1714,33 @@
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="3:3">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="3:3">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:3">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="3:3">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1706,22 +1750,22 @@
       </c>
     </row>
     <row r="20" spans="3:3">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1755,16 +1799,16 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1985,10 +2029,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -2000,164 +2044,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5"/>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="D6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="6">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B7" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B8" s="6" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="6">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
         <v>12</v>
       </c>
-      <c r="B18" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B22" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
         <v>13</v>
       </c>
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+      <c r="B23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+      <c r="B24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
         <v>15</v>
       </c>
-      <c r="B21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+      <c r="B25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
-        <v>114</v>
+      <c r="B26" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2169,37 +2225,64 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="18.75" customWidth="1"/>
     <col min="2" max="2" width="67.125" customWidth="1"/>
+    <col min="3" max="3" width="41.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" t="s">
         <v>118</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" ht="71.25" spans="1:3">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://app.diagrams.net/#G1wKTWF5907AMjdvuFrYsDYcYMQ8MhcJ8H"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.styiens.com/"/>
+    <hyperlink ref="B7" r:id="rId3" display="https://freshdesignweb.com/free-restaurant-coffee-website-templates/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2222,17 +2305,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created landing page(incomplete) app v1.0
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19410" windowHeight="7770" activeTab="4"/>
+    <workbookView windowWidth="19410" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="135">
   <si>
     <t>Todo:</t>
   </si>
@@ -114,18 +114,24 @@
     <t>effects on design</t>
   </si>
   <si>
+    <t>how it works</t>
+  </si>
+  <si>
+    <t>https://cookifi.com/how-it-works</t>
+  </si>
+  <si>
+    <t>ReactStrap designs to implement</t>
+  </si>
+  <si>
+    <t>Carousel</t>
+  </si>
+  <si>
+    <t>https://reactstrap.github.io/components/carousel/</t>
+  </si>
+  <si>
     <t>Bugs to solve:</t>
   </si>
   <si>
-    <t>Add button should be corrected</t>
-  </si>
-  <si>
-    <t>Quantity increase and decrease</t>
-  </si>
-  <si>
-    <t>Reset Button</t>
-  </si>
-  <si>
     <t xml:space="preserve">render the listing of vendor ,customer and transport listing </t>
   </si>
   <si>
@@ -135,6 +141,9 @@
     <t>copy to clipboard button</t>
   </si>
   <si>
+    <t>calculate total and add to order object in database (It is rendered on the front end)</t>
+  </si>
+  <si>
     <t>node APIS fix</t>
   </si>
   <si>
@@ -367,6 +376,15 @@
   </si>
   <si>
     <t>provide feedback</t>
+  </si>
+  <si>
+    <t>Create Contact us page</t>
+  </si>
+  <si>
+    <t>Add messenger chat and chatbot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Map location </t>
   </si>
   <si>
     <t>Flow diagram</t>
@@ -417,9 +435,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -462,19 +480,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,61 +495,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -555,21 +512,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -583,12 +563,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -617,6 +635,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -629,79 +659,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -713,79 +803,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,8 +855,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -855,15 +875,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -900,10 +911,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -917,126 +926,135 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1048,16 +1066,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1452,16 +1470,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C57"/>
+  <dimension ref="A2:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="50.1" customWidth="1"/>
-    <col min="2" max="2" width="29.2" customWidth="1"/>
+    <col min="2" max="2" width="44.375" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1606,72 +1624,86 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="7" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
         <v>31</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
+      <c r="B43" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
+    <row r="57" spans="1:1">
+      <c r="A57" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
         <v>43</v>
       </c>
     </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B40" r:id="rId1" display="https://cookifi.com/how-it-works"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -1683,8 +1715,8 @@
   <sheetPr/>
   <dimension ref="A2:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1696,26 +1728,26 @@
     <row r="2" spans="1:2">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="6"/>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="3:3">
@@ -1751,22 +1783,22 @@
     </row>
     <row r="20" spans="3:3">
       <c r="C20" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1795,228 +1827,228 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2029,10 +2061,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -2046,13 +2078,13 @@
     <row r="1" spans="1:2">
       <c r="A1" s="4"/>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2060,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2068,13 +2100,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2082,10 +2114,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2093,7 +2125,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2101,7 +2133,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2109,7 +2141,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2117,7 +2149,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2125,15 +2157,15 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13">
+      <c r="A13" s="6">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
-        <v>103</v>
+      <c r="B13" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2141,15 +2173,15 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2157,7 +2189,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2165,12 +2197,12 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2178,10 +2210,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2189,7 +2221,7 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2197,7 +2229,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2205,7 +2237,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2213,7 +2245,22 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>115</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2227,8 +2274,8 @@
   <sheetPr/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -2240,42 +2287,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" ht="71.25" spans="1:3">
       <c r="A11" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2305,17 +2352,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
landing page (incomplete) v1.0.1
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19410" windowHeight="7770"/>
+    <workbookView windowWidth="19410" windowHeight="7770" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="Task Details" sheetId="4" r:id="rId4"/>
     <sheet name="Links" sheetId="5" r:id="rId5"/>
     <sheet name="Learning" sheetId="6" r:id="rId6"/>
+    <sheet name="Sell" sheetId="7" r:id="rId7"/>
+    <sheet name="Flow" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="201">
   <si>
     <t>Todo:</t>
   </si>
@@ -123,12 +125,90 @@
     <t>ReactStrap designs to implement</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>where to use</t>
+  </si>
+  <si>
     <t>Carousel</t>
   </si>
   <si>
     <t>https://reactstrap.github.io/components/carousel/</t>
   </si>
   <si>
+    <t>Landing page</t>
+  </si>
+  <si>
+    <t>Alerts</t>
+  </si>
+  <si>
+    <t>To show new messages</t>
+  </si>
+  <si>
+    <t>Badges</t>
+  </si>
+  <si>
+    <t>to show notification</t>
+  </si>
+  <si>
+    <t>Breadcrumbs</t>
+  </si>
+  <si>
+    <t>to show navigations taken by user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collapse </t>
+  </si>
+  <si>
+    <t>for more information to show</t>
+  </si>
+  <si>
+    <t>Fade</t>
+  </si>
+  <si>
+    <t>Fade in fade out animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container </t>
+  </si>
+  <si>
+    <t>for responsive design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modal </t>
+  </si>
+  <si>
+    <t>to show customer oder has been places successfully</t>
+  </si>
+  <si>
+    <t>pagination for items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagination for all items , orders ,customers </t>
+  </si>
+  <si>
+    <t>Progress bar</t>
+  </si>
+  <si>
+    <t>Loading animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spinner </t>
+  </si>
+  <si>
+    <t>tabs</t>
+  </si>
+  <si>
+    <t>to switch between tabs</t>
+  </si>
+  <si>
+    <t>toasts</t>
+  </si>
+  <si>
+    <t>for notifications messages</t>
+  </si>
+  <si>
     <t>Bugs to solve:</t>
   </si>
   <si>
@@ -159,9 +239,6 @@
     <t>in view add update button and delete button</t>
   </si>
   <si>
-    <t>pagination for items</t>
-  </si>
-  <si>
     <t>needs work and testing</t>
   </si>
   <si>
@@ -406,6 +483,12 @@
   </si>
   <si>
     <t>https://freshdesignweb.com/free-restaurant-coffee-website-templates/</t>
+  </si>
+  <si>
+    <t>https://www.templatemonster.com/landing-page-template/plate-healthy-food-one-page-lean-html-landing-page-template-76237.html</t>
+  </si>
+  <si>
+    <t>https://www.templatemonsterpreview.com/demo/58458.html?_gl=1*1exrkr4*_ga*NDc5ODExNDIuMTYwMjk0MzM0NQ..*_ga_FTPYEGT5LY*MTYwOTk0MjkxNy4xLjAuMTYwOTk0MjkyMC41Nw..&amp;_ga=2.77429523.78997421.1609942919-47981142.1602943345</t>
   </si>
   <si>
     <t>Ecommerse site</t>
@@ -421,6 +504,30 @@
 password : 123456</t>
   </si>
   <si>
+    <t>ideas</t>
+  </si>
+  <si>
+    <t>https://in.pinterest.com/search/pins/?q=vegitaren%20food&amp;rs=typed&amp;term_meta[]=vegitaren%7Ctyped&amp;term_meta[]=food%7Ctyped</t>
+  </si>
+  <si>
+    <t>https://www.pizzahut.co.in/</t>
+  </si>
+  <si>
+    <t>https://www.pizzahut.co.in/menu/drinks</t>
+  </si>
+  <si>
+    <t>https://www.pizzahut.co.in/aboutus</t>
+  </si>
+  <si>
+    <t>https://www.zomato.com/bangalore/order-food-online</t>
+  </si>
+  <si>
+    <t>https://www.zomato.com/bangalore/al-amanah-cafe-kammanahalli-bangalore/order</t>
+  </si>
+  <si>
+    <t>https://www.swiggy.com/offers/restaurant</t>
+  </si>
+  <si>
     <t>node backend to link with redux</t>
   </si>
   <si>
@@ -428,6 +535,99 @@
   </si>
   <si>
     <t>responsive design</t>
+  </si>
+  <si>
+    <t>What are the needs to sell this software?</t>
+  </si>
+  <si>
+    <t>Customer should be able to order Food</t>
+  </si>
+  <si>
+    <t>email notification</t>
+  </si>
+  <si>
+    <t>Admin should be able to control Caterer subscriptions</t>
+  </si>
+  <si>
+    <t>Caterer should be able to recieve and manage orders</t>
+  </si>
+  <si>
+    <t>Good looking User Interface</t>
+  </si>
+  <si>
+    <t>Good animations</t>
+  </si>
+  <si>
+    <t>Steps for the flow to work</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Caterer</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Check for authentication</t>
+  </si>
+  <si>
+    <t>View Menu and order food</t>
+  </si>
+  <si>
+    <t>Email Notification</t>
+  </si>
+  <si>
+    <t>order placement</t>
+  </si>
+  <si>
+    <t>order recieved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accept order </t>
+  </si>
+  <si>
+    <t>Email for acceptance</t>
+  </si>
+  <si>
+    <t>accept order</t>
+  </si>
+  <si>
+    <t>Mark on calender</t>
+  </si>
+  <si>
+    <t>Calender and notification</t>
+  </si>
+  <si>
+    <t>Deliver / serve order</t>
+  </si>
+  <si>
+    <t>Generate Bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gets bill </t>
+  </si>
+  <si>
+    <t>generates bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment </t>
+  </si>
+  <si>
+    <t>pays for order</t>
+  </si>
+  <si>
+    <t>Recieves payment</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>provides feedback</t>
   </si>
 </sst>
 </file>
@@ -436,13 +636,20 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -480,8 +687,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,7 +765,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,70 +780,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -587,14 +794,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -635,55 +842,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -695,49 +998,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,67 +1016,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,10 +1062,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -875,6 +1080,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -911,8 +1125,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -926,179 +1142,176 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -1107,7 +1320,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1470,10 +1683,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:C69"/>
+  <dimension ref="A2:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1484,64 +1697,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="13" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1556,7 +1769,7 @@
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1596,13 +1809,13 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1628,76 +1841,181 @@
       <c r="A40" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
+      <c r="C43" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>39</v>
+      <c r="A60" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1726,53 +2044,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="8" t="s">
-        <v>51</v>
+      <c r="C13" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="3:3">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="3:3">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:3">
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="3:3">
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1782,23 +2100,23 @@
       </c>
     </row>
     <row r="20" spans="3:3">
-      <c r="C20" s="9" t="s">
-        <v>52</v>
+      <c r="C20" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="5" t="s">
-        <v>53</v>
+      <c r="B22" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="5" t="s">
-        <v>54</v>
+      <c r="B23" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="5" t="s">
-        <v>55</v>
+      <c r="B24" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1827,228 +2145,228 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>60</v>
+      <c r="A4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2063,8 +2381,8 @@
   <sheetPr/>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -2076,15 +2394,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="4"/>
+      <c r="A1" s="6"/>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="7"/>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2092,56 +2410,56 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="6">
+      <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>96</v>
+      <c r="B6" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>99</v>
+      <c r="B7" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="6">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>101</v>
+      <c r="B8" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>102</v>
+      <c r="B9" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="6">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>103</v>
+      <c r="B10" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2149,7 +2467,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2157,15 +2475,15 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="6">
+      <c r="A13" s="8">
         <v>8</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>106</v>
+      <c r="B13" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2173,15 +2491,15 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2189,7 +2507,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2197,12 +2515,12 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2210,10 +2528,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2221,7 +2539,7 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2229,7 +2547,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2237,7 +2555,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2245,22 +2563,22 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2272,57 +2590,105 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="18.75" customWidth="1"/>
-    <col min="2" max="2" width="67.125" customWidth="1"/>
+    <col min="2" max="2" width="105.75" customWidth="1"/>
     <col min="3" max="3" width="41.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>149</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="2:2">
-      <c r="B7" s="2" t="s">
-        <v>128</v>
+      <c r="B7" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" ht="41" customHeight="1" spans="2:2">
+      <c r="B9" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="11" ht="71.25" spans="1:3">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>131</v>
+        <v>157</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2330,6 +2696,7 @@
     <hyperlink ref="B1" r:id="rId1" display="https://app.diagrams.net/#G1wKTWF5907AMjdvuFrYsDYcYMQ8MhcJ8H"/>
     <hyperlink ref="B4" r:id="rId2" display="https://www.styiens.com/"/>
     <hyperlink ref="B7" r:id="rId3" display="https://freshdesignweb.com/free-restaurant-coffee-website-templates/"/>
+    <hyperlink ref="B8" r:id="rId4" display="https://www.templatemonster.com/landing-page-template/plate-healthy-food-one-page-lean-html-landing-page-template-76237.html" tooltip="https://www.templatemonster.com/landing-page-template/plate-healthy-food-one-page-lean-html-landing-page-template-76237.html"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2352,18 +2719,240 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>134</v>
-      </c>
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="48.625" customWidth="1"/>
+    <col min="2" max="2" width="15.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="3" max="3" width="40.75" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="5" max="5" width="40.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" spans="1:5">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" ht="18" spans="1:5">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" ht="18" spans="1:5">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" ht="18" spans="1:5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" ht="18" spans="1:5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" ht="18" spans="1:5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" ht="18" spans="1:5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" ht="18" spans="1:5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" ht="18" spans="1:5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" ht="18" spans="1:5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
heroku deploy changed axios url
</commit_message>
<xml_diff>
--- a/Aaswad Caterers.xlsx
+++ b/Aaswad Caterers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19410" windowHeight="7770" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="19410" windowHeight="7770" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="209">
   <si>
     <t>Todo:</t>
   </si>
@@ -383,6 +383,9 @@
     <t>In progress</t>
   </si>
   <si>
+    <t>Important</t>
+  </si>
+  <si>
     <t>Requirements and Analysis</t>
   </si>
   <si>
@@ -462,6 +465,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add Map location </t>
+  </si>
+  <si>
+    <t>Deploy the App</t>
   </si>
   <si>
     <t>Flow diagram</t>
@@ -528,6 +534,12 @@
     <t>https://www.swiggy.com/offers/restaurant</t>
   </si>
   <si>
+    <t>https://www.etsy.com/</t>
+  </si>
+  <si>
+    <t>https://blog.hubspot.com/marketing/mobile-website-design-examples</t>
+  </si>
+  <si>
     <t>node backend to link with redux</t>
   </si>
   <si>
@@ -535,6 +547,18 @@
   </si>
   <si>
     <t>responsive design</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/css/exercise.asp?filename=exercise_background3</t>
+  </si>
+  <si>
+    <t>https://classroom.udacity.com/courses/ud001/lessons/6987421963/concepts/5dbe066a-c5a4-47e2-bc1b-9e56f2e05b7e</t>
+  </si>
+  <si>
+    <t>https://medium.com/codex/harvards-most-popular-course-is-free-online-283301b6c531</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ngc9gnGgUdA&amp;ab_channel=JavaScriptMastery</t>
   </si>
   <si>
     <t>What are the needs to sell this software?</t>
@@ -635,12 +659,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,9 +703,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -695,71 +763,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -771,23 +779,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -807,15 +807,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -836,187 +874,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1045,6 +1089,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1056,39 +1109,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1123,13 +1143,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1142,147 +1175,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1292,7 +1336,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1317,16 +1361,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1697,64 +1750,64 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1769,7 +1822,7 @@
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1809,13 +1862,13 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="12" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1964,7 +2017,7 @@
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="12" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2050,7 +2103,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>73</v>
       </c>
@@ -2064,33 +2117,33 @@
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="3:3">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="3:3">
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:3">
-      <c r="B16" s="12"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:3">
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="3:3">
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="14" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2100,7 +2153,7 @@
       </c>
     </row>
     <row r="20" spans="3:3">
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="14" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2149,16 +2202,16 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2379,10 +2432,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelCol="3"/>
@@ -2405,61 +2458,67 @@
         <v>119</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="8">
+      <c r="A6" s="10">
         <v>1</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>121</v>
+      <c r="B6" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="8">
+      <c r="A7" s="10">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>124</v>
+      <c r="B7" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8">
+      <c r="A8" s="10">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>126</v>
+      <c r="B8" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8">
+      <c r="A9" s="10">
         <v>4</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>127</v>
+      <c r="B9" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="8">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>128</v>
+      <c r="B10" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2467,7 +2526,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2475,15 +2534,15 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8">
+      <c r="A13" s="10">
         <v>8</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>131</v>
+      <c r="B13" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2491,15 +2550,15 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2507,7 +2566,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2515,12 +2574,12 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2528,10 +2587,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2539,7 +2598,7 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2547,7 +2606,7 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2555,7 +2614,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2563,22 +2622,27 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2590,10 +2654,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -2605,90 +2669,100 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" ht="41" customHeight="1" spans="2:2">
       <c r="B9" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" ht="71.25" spans="1:3">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>166</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2706,30 +2780,50 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="28.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2755,35 +2849,35 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2813,16 +2907,16 @@
     <row r="1" ht="18" spans="1:5">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" ht="18" spans="1:5">
@@ -2830,16 +2924,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" ht="18" spans="1:5">
@@ -2847,13 +2941,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -2862,13 +2956,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -2877,13 +2971,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -2892,11 +2986,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -2905,7 +2999,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2916,13 +3010,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2931,13 +3025,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -2946,10 +3040,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>

</xml_diff>